<commit_message>
Actualización de plantilla de tasación muĺtiple
</commit_message>
<xml_diff>
--- a/assets/plantilla_tasacion_basica.xlsx
+++ b/assets/plantilla_tasacion_basica.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alejandro\proyectos\ASDIH-AESVAL-POC-code\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejandro.garnung\Documents\ASDIH\AESVAL\ASDIH-AESVAL-POC-code\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28680" windowHeight="11066"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17229"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>codigo_municipio</t>
   </si>
@@ -42,34 +42,28 @@
     <t>vivienda_nueva</t>
   </si>
   <si>
-    <t>antiguedad</t>
-  </si>
-  <si>
-    <t>rehabilitacion</t>
-  </si>
-  <si>
     <t>calidad_alta</t>
   </si>
   <si>
-    <t>estado_conservacion</t>
-  </si>
-  <si>
-    <t>Buena</t>
-  </si>
-  <si>
     <t>FALSE</t>
   </si>
   <si>
-    <t>TRUE</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>error_intencionado</t>
   </si>
   <si>
-    <t>Muy deficiente</t>
+    <t>calefaccion</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>creci</t>
+  </si>
+  <si>
+    <t>renta</t>
   </si>
 </sst>
 </file>
@@ -438,8 +432,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -449,10 +443,8 @@
     <col min="3" max="3" width="16.921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.07421875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.3828125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
@@ -481,13 +473,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
@@ -507,22 +499,22 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -547,17 +539,17 @@
       <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>15</v>
+      <c r="H3" t="b">
+        <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -568,7 +560,7 @@
         <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -582,17 +574,17 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>15</v>
-      </c>
-      <c r="I4">
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="b">
         <v>1</v>
       </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -612,22 +604,22 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>15</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>11</v>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>